<commit_message>
feat(tasks): standardize prompt JSON blocks and add h-001/h-002 assets
</commit_message>
<xml_diff>
--- a/data-warehouse/human-generated/MRW-LBO-Model-No-Circ.xlsx
+++ b/data-warehouse/human-generated/MRW-LBO-Model-No-Circ.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52E018E-18AA-4251-88A2-9892023AE6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179FCE3A-05DA-4C2D-99B2-0B365EC07BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22875" windowHeight="14431" xr2:uid="{86AD583E-3221-4694-9BB1-CC8A811C0A53}"/>
+    <workbookView xWindow="-98" yWindow="353" windowWidth="28996" windowHeight="15944" activeTab="1" xr2:uid="{86AD583E-3221-4694-9BB1-CC8A811C0A53}"/>
   </bookViews>
   <sheets>
-    <sheet name="Operating Model" sheetId="1" r:id="rId1"/>
+    <sheet name="1. Business Assessment" sheetId="2" r:id="rId1"/>
+    <sheet name="Operating Model" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="CIQWBGuid" hidden="1">"ad3d7874-e656-4b70-85f6-774c057cde64"</definedName>
@@ -42,8 +43,9 @@
     <definedName name="IQ_WEEK">50000</definedName>
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Operating Model'!$B$2:$U$208</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Operating Model'!$2:$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'1. Business Assessment'!$B$2:$W$69</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operating Model'!$B$2:$U$208</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Operating Model'!$2:$19</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="autoNoTable" iterate="1"/>
   <extLst>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="164">
   <si>
     <t>D&amp;A</t>
   </si>
@@ -421,6 +423,141 @@
   </si>
   <si>
     <t>Model</t>
+  </si>
+  <si>
+    <t>Q1: Business Assessment</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>Do NOT invest in this business on account of an unfavourable risk-reward:</t>
+  </si>
+  <si>
+    <t>Low base case returns, extremely sensitive to changes in COGS spend and revenue/store. Bulk of returns driven by EBITDA growth, which will require a lot of conviction / potential portfolio management</t>
+  </si>
+  <si>
+    <t>Cannot lever up much as a result</t>
+  </si>
+  <si>
+    <t>Complete wipe-out of returns in a relatively mild downside case (e.g. not assuming a business collapse)</t>
+  </si>
+  <si>
+    <t>Potential remedies include ability to enter at a more attractive valuation or new value creation levers to make the base case more compelling</t>
+  </si>
+  <si>
+    <t>Strengths</t>
+  </si>
+  <si>
+    <t>#1 net promoter score and brand warmth, increased traffic from Fresh Look marketing initiative</t>
+  </si>
+  <si>
+    <t>3rd lowest exposure to food delivery growth in spheres of influence among UK supermarkets</t>
+  </si>
+  <si>
+    <t>Captive fuel revenues diversify revenue streams</t>
+  </si>
+  <si>
+    <t>Low capital intensity (capex spend did not meaningfully increase despite store openings during COVID)</t>
+  </si>
+  <si>
+    <t>Negative NWC business model is a source of cash as the business grows</t>
+  </si>
+  <si>
+    <t>Weaknesses</t>
+  </si>
+  <si>
+    <t>Traditionally limited pricing power in the industry as supermarkets compete aggressively on price</t>
+  </si>
+  <si>
+    <t>Low margin profile (~80% COGS) and very high sensitivity with potentially limited control over key drivers, such as transportation costs given supplier consolidation</t>
+  </si>
+  <si>
+    <t>High exposure (12% of sales) to employee costs in a tight labour market. # of FTEs has rebounded and even before COVID, staff reductions started to taper</t>
+  </si>
+  <si>
+    <t>Weak FCF conversion (40% pre-COVID). ~3% capex spend appears to significantly exceed that of the industry (0.5% sales)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limited downside protection in the event of a downturn - negative FCF in FY21 </t>
+  </si>
+  <si>
+    <t>Opportunities</t>
+  </si>
+  <si>
+    <t>Drive up-sell of customers beyond groceries and fuel (e.g. higher-margin leisure/dining activities). Also greater penetration of fuel sales</t>
+  </si>
+  <si>
+    <t>Good traction with online sales (3x increase last year)</t>
+  </si>
+  <si>
+    <t>Vertical integration - opportunity to drive margins</t>
+  </si>
+  <si>
+    <t>Currently under-penetrated in the ready meal category, which is experiencing strong growth</t>
+  </si>
+  <si>
+    <t>Threats</t>
+  </si>
+  <si>
+    <t>Aggressive competition from "discounters" (86% already located next to a Morrison's and potential continuation). Gradual market share erosion since 2012</t>
+  </si>
+  <si>
+    <t>Food delivery platforms offering grocery deliveries, such as Deliveroo</t>
+  </si>
+  <si>
+    <t>Potential rebound of food service vs. retail consumption</t>
+  </si>
+  <si>
+    <t>Need to invest in capex to repurpose petrol stations into EV charging points</t>
+  </si>
+  <si>
+    <t>Investment Highlights</t>
+  </si>
+  <si>
+    <t>Core demand for groceries is generally recession-proof (~2% growth during GFC) and tends to outperform in downturns (as consumers shift consumption paterns)</t>
+  </si>
+  <si>
+    <t>Structural growth drivers following COVID - 1Q22 sales up despite tough COVID comps</t>
+  </si>
+  <si>
+    <t>Barriers to entry for new supermarket entrants, such as real estate and brand value which Morrison's has</t>
+  </si>
+  <si>
+    <t>Value creation levers: commercial (e.g. Fresh look initiative), operational (e.g. employee rationalisation, vertical integration)</t>
+  </si>
+  <si>
+    <t>Risks for Further DD</t>
+  </si>
+  <si>
+    <t>UK supermarket TAM and how it is expected to evolve</t>
+  </si>
+  <si>
+    <t>Online grocery TAM, penetration and Morrison's KPIs. How strong are in-house capabilities and how reliant is the business on external partners like Amazon?</t>
+  </si>
+  <si>
+    <t>Validation of vertical integration strategy and potential white spaces</t>
+  </si>
+  <si>
+    <t>Channel checks: customer surveys, employee interviews</t>
+  </si>
+  <si>
+    <t>Management's go-forward strategy</t>
+  </si>
+  <si>
+    <t>Cost of sales - contribution margins by segment/category</t>
+  </si>
+  <si>
+    <t>Other costs are 5% of sales - need to figure out the composition and gain comfort that they are a constant % of sales</t>
+  </si>
+  <si>
+    <t>Figure out maintenance vs. expansionary capex split and drivers</t>
+  </si>
+  <si>
+    <t>Expansionary capex for petrol stations vs stores, also taking EV transition into account</t>
+  </si>
+  <si>
+    <t>Ability to structure an investment with more downside protection, e.g. 1x liq pref convertible preferred stock</t>
   </si>
 </sst>
 </file>
@@ -688,7 +825,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,6 +913,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF007000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1281,7 +1424,7 @@
     <xf numFmtId="178" fontId="28" fillId="12" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="179" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="232">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1870,6 +2013,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="15" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Bad" xfId="2" builtinId="27" hidden="1"/>
@@ -2215,11 +2362,547 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E0DBB2-E856-4409-A4E7-F6E75D790A28}">
+  <dimension ref="C1:L56"/>
+  <sheetViews>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="3" width="1.73046875" customWidth="1"/>
+    <col min="4" max="12" width="9.265625" customWidth="1"/>
+    <col min="13" max="13" width="1.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:12" ht="9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="3:12" ht="9" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="3" spans="3:12" ht="24" x14ac:dyDescent="0.85">
+      <c r="C3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="3:12" ht="3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="3:12" ht="3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" s="230"/>
+      <c r="D5" s="230"/>
+      <c r="E5" s="230"/>
+      <c r="F5" s="230"/>
+      <c r="G5" s="231"/>
+      <c r="H5" s="231"/>
+      <c r="I5" s="231"/>
+      <c r="J5" s="231"/>
+      <c r="K5" s="231"/>
+      <c r="L5" s="231"/>
+    </row>
+    <row r="6" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D10" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D14" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D21" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D22" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D24" t="s">
+        <v>135</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D25" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D26" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D28" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D29" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D30" t="s">
+        <v>140</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D31" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D32" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D34" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D35" t="s">
+        <v>144</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D36" t="s">
+        <v>145</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D37" t="s">
+        <v>146</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D38" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D40" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D41" t="s">
+        <v>149</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D42" t="s">
+        <v>150</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D43" t="s">
+        <v>151</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D44" t="s">
+        <v>152</v>
+      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="4:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="4:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="D46" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="4:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="D47" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="4:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="D48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D49" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D50" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D51" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D52" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D53" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D54" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D56" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="52" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42283070-E20D-476D-846B-3C941E250C86}">
   <dimension ref="A1:AB240"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="88" zoomScaleNormal="88" zoomScaleSheetLayoutView="88" workbookViewId="0">
-      <selection activeCell="P78" sqref="P78"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="88" zoomScaleNormal="88" zoomScaleSheetLayoutView="88" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2355,7 +3038,7 @@
         <v>92</v>
       </c>
       <c r="F9" s="142">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="116"/>
@@ -2377,7 +3060,7 @@
       <c r="O9" s="39"/>
       <c r="R9" s="93">
         <f>+F12</f>
-        <v>4705.3500000000004</v>
+        <v>5332.73</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="17.649999999999999" x14ac:dyDescent="0.85">
@@ -2440,7 +3123,7 @@
       <c r="O11" s="39"/>
       <c r="R11" s="97">
         <f>+R12*F14</f>
-        <v>65.413499999999999</v>
+        <v>71.687299999999993</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="17.649999999999999" x14ac:dyDescent="0.85">
@@ -2453,7 +3136,7 @@
       <c r="E12" s="59"/>
       <c r="F12" s="140">
         <f>+F9*(1+F10)*F11/100</f>
-        <v>4705.3500000000004</v>
+        <v>5332.73</v>
       </c>
       <c r="H12"/>
       <c r="I12" s="91" t="s">
@@ -2462,11 +3145,11 @@
       <c r="J12" s="39"/>
       <c r="K12" s="97">
         <f>$R$13-K9</f>
-        <v>3429.7635</v>
+        <v>4063.4172999999992</v>
       </c>
       <c r="L12" s="196">
         <f>K12/$J$107</f>
-        <v>4.8580219546742214</v>
+        <v>5.7555485835694036</v>
       </c>
       <c r="M12"/>
       <c r="N12" s="120" t="s">
@@ -2497,11 +3180,11 @@
       <c r="J13" s="99"/>
       <c r="K13" s="96">
         <f>+K9+K12</f>
-        <v>6606.7635</v>
+        <v>7240.4172999999992</v>
       </c>
       <c r="L13" s="197">
         <f>K13/$J$107</f>
-        <v>9.3580219546742214</v>
+        <v>10.255548583569404</v>
       </c>
       <c r="M13"/>
       <c r="N13" s="98" t="s">
@@ -2512,7 +3195,7 @@
       <c r="Q13" s="99"/>
       <c r="R13" s="96">
         <f>SUM(R9:R11)</f>
-        <v>6606.7635</v>
+        <v>7240.4172999999992</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -2525,7 +3208,7 @@
       <c r="E14" s="14"/>
       <c r="F14" s="96">
         <f>+F12+F13</f>
-        <v>6541.35</v>
+        <v>7168.73</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14"/>
@@ -2548,7 +3231,7 @@
       <c r="E15" s="118"/>
       <c r="F15" s="119">
         <f>+F14/$K$107</f>
-        <v>7.9044359068124868</v>
+        <v>8.6625492930731234</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15"/>
@@ -2557,7 +3240,7 @@
       </c>
       <c r="J15" s="211">
         <f>F205</f>
-        <v>0.19431033730506894</v>
+        <v>0.15451559424400332</v>
       </c>
       <c r="K15"/>
       <c r="L15"/>
@@ -2584,7 +3267,7 @@
       <c r="E16" s="199"/>
       <c r="F16" s="200">
         <f>+F14/$J$107</f>
-        <v>9.2653682719546744</v>
+        <v>10.154008498583568</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16"/>
@@ -2593,7 +3276,7 @@
       </c>
       <c r="J16" s="213">
         <f>F206</f>
-        <v>2.4310686964511681</v>
+        <v>2.0519651479263024</v>
       </c>
       <c r="K16"/>
       <c r="L16"/>
@@ -8194,7 +8877,7 @@
       <c r="I192" s="202"/>
       <c r="J192" s="135">
         <f>$L$13</f>
-        <v>9.3580219546742214</v>
+        <v>10.255548583569404</v>
       </c>
       <c r="K192" s="80">
         <v>10</v>
@@ -8230,7 +8913,7 @@
       <c r="I193" s="81"/>
       <c r="J193" s="61">
         <f t="shared" ref="J193" si="112">J191*J192</f>
-        <v>6606.7635</v>
+        <v>7240.4172999999992</v>
       </c>
       <c r="K193" s="60">
         <f>K191*K192</f>
@@ -8313,7 +8996,7 @@
       <c r="I196" s="84"/>
       <c r="J196" s="136">
         <f t="shared" ref="J196:O196" si="115">J193+J195</f>
-        <v>3429.7635</v>
+        <v>4063.4172999999992</v>
       </c>
       <c r="K196" s="85">
         <f t="shared" si="115"/>
@@ -8403,7 +9086,7 @@
       <c r="I199" s="27"/>
       <c r="J199" s="61">
         <f t="shared" ref="J199" si="117">J196+J198</f>
-        <v>3429.7635</v>
+        <v>4063.4172999999992</v>
       </c>
       <c r="K199" s="60">
         <f>K196+K198</f>
@@ -8464,7 +9147,7 @@
       <c r="I203" s="25"/>
       <c r="J203" s="64">
         <f>-J199</f>
-        <v>-3429.7635</v>
+        <v>-4063.4172999999992</v>
       </c>
       <c r="K203" s="17">
         <f>K$199*(K19=$F$203)</f>
@@ -8500,7 +9183,7 @@
       <c r="E205" s="72"/>
       <c r="F205" s="86">
         <f>IFERROR(XIRR(J203:O203,J19:O19),"n/a")</f>
-        <v>0.19431033730506894</v>
+        <v>0.15451559424400332</v>
       </c>
       <c r="O205" s="17"/>
       <c r="R205"/>
@@ -8513,7 +9196,7 @@
       <c r="E206" s="74"/>
       <c r="F206" s="87">
         <f>-SUM(K203:O203)/J203</f>
-        <v>2.4310686964511681</v>
+        <v>2.0519651479263024</v>
       </c>
     </row>
     <row r="207" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
@@ -8524,7 +9207,7 @@
       <c r="E207" s="76"/>
       <c r="F207" s="88">
         <f>SUM(K203:O203)+J203</f>
-        <v>4908.2271810807952</v>
+        <v>4274.573381080796</v>
       </c>
     </row>
     <row r="208" spans="3:18" x14ac:dyDescent="0.55000000000000004">

</xml_diff>